<commit_message>
Updated comments and added helper files
</commit_message>
<xml_diff>
--- a/input_sample.xlsx
+++ b/input_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\MATLAB_FEM_Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD08472-4C06-430F-BC67-6B54BF0D80C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2E4AF7-5F96-4737-B525-5EF8FFADC64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="3348" windowWidth="17280" windowHeight="8964" xr2:uid="{BF58F311-CE55-47BF-8057-1A0B2460D30F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BF58F311-CE55-47BF-8057-1A0B2460D30F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>element</t>
   </si>
@@ -115,6 +115,24 @@
   </si>
   <si>
     <t>The force acting on the node in the y-direction (Fy)</t>
+  </si>
+  <si>
+    <t>node15</t>
+  </si>
+  <si>
+    <t>node16</t>
+  </si>
+  <si>
+    <t>node17</t>
+  </si>
+  <si>
+    <t>node18</t>
+  </si>
+  <si>
+    <t>node19</t>
+  </si>
+  <si>
+    <t>node20</t>
   </si>
 </sst>
 </file>
@@ -524,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DBEDF8-66C2-4673-BC3F-61A0C7F26D30}">
   <dimension ref="A1:AL30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,12 +631,24 @@
       <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
+      <c r="Y1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -632,446 +662,194 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>4</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H2" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="O2" s="1">
-        <v>3</v>
-      </c>
-      <c r="P2" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="R2" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="S2" s="1">
-        <v>6</v>
-      </c>
-      <c r="T2" s="1">
-        <v>6</v>
-      </c>
-      <c r="U2" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="V2" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="W2" s="1">
-        <v>9</v>
-      </c>
-      <c r="X2" s="1">
-        <v>9</v>
-      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H3" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>1</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>1</v>
-      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>6</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H4" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1">
-        <v>0</v>
-      </c>
-      <c r="V4" s="1">
-        <v>0</v>
-      </c>
-      <c r="W4" s="1">
-        <v>100000</v>
-      </c>
-      <c r="X4" s="1">
-        <v>-100000</v>
-      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H5" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0</v>
-      </c>
-      <c r="V5" s="1">
-        <v>0</v>
-      </c>
-      <c r="W5" s="1">
-        <v>0</v>
-      </c>
-      <c r="X5" s="1">
-        <v>0</v>
-      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1">
-        <v>8</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H6" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0</v>
-      </c>
-      <c r="T6" s="1">
-        <v>0</v>
-      </c>
-      <c r="U6" s="1">
-        <v>0</v>
-      </c>
-      <c r="V6" s="1">
-        <v>0</v>
-      </c>
-      <c r="W6" s="1">
-        <v>0</v>
-      </c>
-      <c r="X6" s="1">
-        <v>0</v>
-      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1">
-        <v>7</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H7" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1">
-        <v>0</v>
-      </c>
-      <c r="U7" s="1">
-        <v>0</v>
-      </c>
-      <c r="V7" s="1">
-        <v>0</v>
-      </c>
-      <c r="W7" s="1">
-        <v>0</v>
-      </c>
-      <c r="X7" s="1">
-        <v>0</v>
-      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>10</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H8" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1081,26 +859,14 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>9</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H9" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1113,26 +879,14 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1">
-        <v>12</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H10" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
@@ -1142,79 +896,45 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1">
-        <v>11</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H11" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1">
-        <v>14</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H12" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1">
-        <v>13</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="H13" s="2">
-        <v>200000000000</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.35</v>
-      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1225,7 +945,9 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1236,7 +958,9 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1247,7 +971,9 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1258,7 +984,9 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1269,7 +997,9 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1281,7 +1011,9 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1293,7 +1025,9 @@
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>

</xml_diff>